<commit_message>
small updates to documentation spreadsheet
</commit_message>
<xml_diff>
--- a/documentation/NCW Epi Dashboards_indicator information.xlsx
+++ b/documentation/NCW Epi Dashboards_indicator information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amoli\OneDrive\Documents\GitHub\ncw_dashboards\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A81867F-9291-4085-B6DB-127F8B4CDE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4C29B2-CCCB-4D37-B262-7313AD695E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -348,9 +348,6 @@
   </si>
   <si>
     <t>None</t>
-  </si>
-  <si>
-    <t>Individual Counties (no regional OR state data available)_</t>
   </si>
   <si>
     <t>Rate per 1,000 housholds</t>
@@ -1069,6 +1066,9 @@
   </si>
   <si>
     <t xml:space="preserve">Due to small numbers in the NCW Epi counties, values in the official PIT Count data were suppressed at times (any value &lt;11 or values that could lead to identification of small numbers). Because of this, some values provided in this dashboard are estimates. See the PIT Count website for more information on how data  are collected. </t>
+  </si>
+  <si>
+    <t>Individual Counties (no regional OR state data available)</t>
   </si>
 </sst>
 </file>
@@ -1434,8 +1434,8 @@
   </sheetPr>
   <dimension ref="A1:L999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H17" zoomScale="97" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1483,13 +1483,13 @@
         <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>86</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="51.5" x14ac:dyDescent="0.3">
@@ -1522,10 +1522,10 @@
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="51.5" x14ac:dyDescent="0.3">
@@ -1558,10 +1558,10 @@
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="51.5" x14ac:dyDescent="0.3">
@@ -1594,10 +1594,10 @@
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="12" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
@@ -1653,10 +1653,10 @@
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="38.5" x14ac:dyDescent="0.3">
@@ -1679,7 +1679,7 @@
         <v>95</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>97</v>
@@ -1689,10 +1689,10 @@
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="50.5" x14ac:dyDescent="0.3">
@@ -1725,10 +1725,10 @@
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="60.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1761,10 +1761,10 @@
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="122" customHeight="1" x14ac:dyDescent="0.3">
@@ -1797,10 +1797,10 @@
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="180" x14ac:dyDescent="0.3">
@@ -1831,10 +1831,10 @@
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="17" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
@@ -1951,7 +1951,7 @@
         <v>91</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>104</v>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="51.5" x14ac:dyDescent="0.25">
@@ -1987,20 +1987,20 @@
         <v>92</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>65</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>66</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="75.5" x14ac:dyDescent="0.3">
@@ -2014,28 +2014,28 @@
         <v>2021</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>92</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>75</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>76</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="75.5" x14ac:dyDescent="0.3">
@@ -2049,28 +2049,28 @@
         <v>2021</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>92</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>23</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>78</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="75.5" x14ac:dyDescent="0.3">
@@ -2084,7 +2084,7 @@
         <v>2021</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>92</v>
@@ -2096,16 +2096,16 @@
         <v>25</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>79</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="50.5" x14ac:dyDescent="0.3">
@@ -2122,7 +2122,7 @@
         <v>91</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>104</v>
@@ -2138,7 +2138,7 @@
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="100" x14ac:dyDescent="0.25">
@@ -2161,19 +2161,19 @@
         <v>104</v>
       </c>
       <c r="G22" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>68</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -2199,14 +2199,14 @@
         <v>28</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>84</v>
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -2217,7 +2217,7 @@
         <v>83</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>91</v>
@@ -2232,14 +2232,14 @@
         <v>30</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>85</v>
       </c>
       <c r="J24" s="6"/>
       <c r="K24" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="50.5" x14ac:dyDescent="0.3">
@@ -2250,29 +2250,29 @@
         <v>70</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>92</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>71</v>
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="50.5" x14ac:dyDescent="0.3">
@@ -2283,29 +2283,29 @@
         <v>70</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>92</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>72</v>
       </c>
       <c r="J26" s="6"/>
       <c r="K26" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
andrea final updates to documentation
</commit_message>
<xml_diff>
--- a/documentation/NCW Epi Dashboards_indicator information.xlsx
+++ b/documentation/NCW Epi Dashboards_indicator information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amoli\OneDrive\Documents\GitHub\ncw_dashboards\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4C29B2-CCCB-4D37-B262-7313AD695E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D095E53A-2AAF-4FE5-9C03-BA83432DB145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="149">
   <si>
     <t>Diabetes</t>
   </si>
@@ -830,9 +830,6 @@
     </r>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>The reference for CHAT data are included directly in the data download spreadsheet, refer to that for dates</t>
   </si>
   <si>
@@ -1070,12 +1067,134 @@
   <si>
     <t>Individual Counties (no regional OR state data available)</t>
   </si>
+  <si>
+    <t>As of June 2024, UW team was not able to gain access to this data source. If there is interest in creating this dashboard, see the NCW EPI Dashboard data download and cleaning instructions</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">U.S. Census Bureau. Types of Health Insurance Coverage by Age. American Community Survey, ACS 5-Year Estimates Detailed Tables, Table B27010. Retrieved </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA ACCESSED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, from
+https://data.census.gov/table/ACSDT1Y2022.B27010?q=B27010</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">U.S. Census Bureau. Receipt of Food Stamps/SNAP in the Past 12 Months by Disability Status for Households. American Community Survey, ACS 5-Year Estimates Detailed Tables, Table B22010. Retrieved </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA ACCESS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, from
+https://data.census.gov/table/ACSDT1Y2022.B22010?q=B22010</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">U.S. Census Bureau.  Poverty Status in the Past 12 Months by Age by Language Spoken at Home for the Population 5 Years and Over. American Community Survey, ACS 5-Year Estimates Detailed Tables, Table B16009. Retrieved </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA ACCESS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, from https://data.census.gov/table/ACSDT1Y2022.B16009?q=B16009</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">U.S. Census Bureau. Employment Status by Disability Status. American Community Survey, ACS 5-Year Estimates Detailed Tables, Table C18120. Retrieved </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSERT DATE OF DATA ACCESS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, from
+https://data.census.gov/table/ACSDT1Y2022.C18120?q=C18120.</t>
+    </r>
+  </si>
+  <si>
+    <t>Stratifications may be possible, see ACS documenatation for variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pregnancies per 1,000 </t>
+  </si>
+  <si>
+    <t>Yearly (goes by school year)</t>
+  </si>
+  <si>
+    <t>Other Dashboard Notes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1131,8 +1250,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1142,12 +1268,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1164,7 +1284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1193,18 +1313,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1214,6 +1322,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1435,7 +1558,7 @@
   <dimension ref="A1:L999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1483,13 +1606,13 @@
         <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="20" t="s">
-        <v>126</v>
+      <c r="L1" s="14" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="51.5" x14ac:dyDescent="0.3">
@@ -1521,11 +1644,11 @@
         <v>37</v>
       </c>
       <c r="J2" s="6"/>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="L2" s="19" t="s">
-        <v>127</v>
+      <c r="L2" s="13" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="51.5" x14ac:dyDescent="0.3">
@@ -1557,11 +1680,11 @@
         <v>39</v>
       </c>
       <c r="J3" s="6"/>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="L3" s="19" t="s">
-        <v>127</v>
+      <c r="L3" s="13" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="51.5" x14ac:dyDescent="0.3">
@@ -1593,14 +1716,14 @@
         <v>41</v>
       </c>
       <c r="J4" s="6"/>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="L4" s="19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="12" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="L4" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>42</v>
       </c>
@@ -1622,6 +1745,9 @@
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="11"/>
+      <c r="L5" s="11" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="38.5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -1652,11 +1778,11 @@
         <v>45</v>
       </c>
       <c r="J6" s="6"/>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="L6" s="19" t="s">
-        <v>127</v>
+      <c r="L6" s="13" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="38.5" x14ac:dyDescent="0.3">
@@ -1679,7 +1805,7 @@
         <v>95</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>97</v>
@@ -1688,11 +1814,11 @@
         <v>46</v>
       </c>
       <c r="J7" s="6"/>
-      <c r="K7" s="19" t="s">
+      <c r="K7" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="L7" s="19" t="s">
-        <v>127</v>
+      <c r="L7" s="13" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="50.5" x14ac:dyDescent="0.3">
@@ -1724,11 +1850,11 @@
         <v>48</v>
       </c>
       <c r="J8" s="6"/>
-      <c r="K8" s="19" t="s">
+      <c r="K8" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="L8" s="19" t="s">
-        <v>127</v>
+      <c r="L8" s="13" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="60.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1760,11 +1886,11 @@
         <v>50</v>
       </c>
       <c r="J9" s="6"/>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="L9" s="19" t="s">
-        <v>127</v>
+      <c r="L9" s="13" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="122" customHeight="1" x14ac:dyDescent="0.3">
@@ -1796,11 +1922,11 @@
         <v>52</v>
       </c>
       <c r="J10" s="6"/>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="L10" s="19" t="s">
-        <v>127</v>
+      <c r="L10" s="13" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="180" x14ac:dyDescent="0.3">
@@ -1825,117 +1951,151 @@
       <c r="G11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="13" t="s">
+        <v>146</v>
+      </c>
       <c r="I11" s="6" t="s">
         <v>54</v>
       </c>
       <c r="J11" s="6"/>
-      <c r="K11" s="19" t="s">
+      <c r="K11" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="L11" s="19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="17" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="L11" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="18" customFormat="1" ht="50.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13" t="s">
+      <c r="C12" s="15">
+        <v>2022</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14" t="s">
+      <c r="E12" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="J12" s="15"/>
-      <c r="K12" s="16"/>
-    </row>
-    <row r="13" spans="1:12" s="17" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="J12" s="17"/>
+      <c r="K12" s="20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="18" customFormat="1" ht="63.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13" t="s">
+      <c r="C13" s="15">
+        <v>2022</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14" t="s">
+      <c r="E13" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="G13" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="J13" s="15"/>
-      <c r="K13" s="16"/>
-    </row>
-    <row r="14" spans="1:12" s="17" customFormat="1" ht="50" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="J13" s="17"/>
+      <c r="K13" s="20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="18" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13" t="s">
+      <c r="C14" s="15">
+        <v>2022</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14" t="s">
+      <c r="E14" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="G14" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="16"/>
-    </row>
-    <row r="15" spans="1:12" s="17" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="J14" s="17"/>
+      <c r="K14" s="20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="18" customFormat="1" ht="50.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13" t="s">
+      <c r="C15" s="15">
+        <v>2022</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14" t="s">
+      <c r="E15" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="G15" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="16"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="20" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="46" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
@@ -1951,7 +2111,7 @@
         <v>91</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>104</v>
@@ -1966,8 +2126,8 @@
         <v>62</v>
       </c>
       <c r="J16" s="6"/>
-      <c r="K16" s="19" t="s">
-        <v>128</v>
+      <c r="K16" s="13" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="51.5" x14ac:dyDescent="0.25">
@@ -1999,8 +2159,8 @@
         <v>66</v>
       </c>
       <c r="J17" s="6"/>
-      <c r="K17" s="19" t="s">
-        <v>129</v>
+      <c r="K17" s="13" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="75.5" x14ac:dyDescent="0.3">
@@ -2032,10 +2192,10 @@
         <v>76</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="K18" s="19" t="s">
-        <v>130</v>
+        <v>137</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="75.5" x14ac:dyDescent="0.3">
@@ -2067,10 +2227,10 @@
         <v>78</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>130</v>
+        <v>137</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="75.5" x14ac:dyDescent="0.3">
@@ -2102,10 +2262,10 @@
         <v>79</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>130</v>
+        <v>137</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="50.5" x14ac:dyDescent="0.3">
@@ -2122,7 +2282,7 @@
         <v>91</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>104</v>
@@ -2137,8 +2297,8 @@
         <v>82</v>
       </c>
       <c r="J21" s="6"/>
-      <c r="K21" s="19" t="s">
-        <v>131</v>
+      <c r="K21" s="13" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="100" x14ac:dyDescent="0.25">
@@ -2170,10 +2330,10 @@
         <v>68</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="K22" s="19" t="s">
-        <v>132</v>
+        <v>138</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -2183,7 +2343,7 @@
       <c r="B23" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="12">
         <v>2021</v>
       </c>
       <c r="D23" s="4" t="s">
@@ -2205,8 +2365,8 @@
         <v>84</v>
       </c>
       <c r="J23" s="6"/>
-      <c r="K23" s="19" t="s">
-        <v>133</v>
+      <c r="K23" s="13" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -2216,11 +2376,11 @@
       <c r="B24" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>91</v>
+      <c r="D24" s="21" t="s">
+        <v>147</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>92</v>
@@ -2238,8 +2398,8 @@
         <v>85</v>
       </c>
       <c r="J24" s="6"/>
-      <c r="K24" s="19" t="s">
-        <v>134</v>
+      <c r="K24" s="13" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="50.5" x14ac:dyDescent="0.3">
@@ -2249,7 +2409,7 @@
       <c r="B25" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="12" t="s">
         <v>119</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -2271,8 +2431,8 @@
         <v>71</v>
       </c>
       <c r="J25" s="6"/>
-      <c r="K25" s="19" t="s">
-        <v>135</v>
+      <c r="K25" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="50.5" x14ac:dyDescent="0.3">
@@ -2282,7 +2442,7 @@
       <c r="B26" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="12" t="s">
         <v>119</v>
       </c>
       <c r="D26" s="4" t="s">
@@ -2304,8 +2464,8 @@
         <v>72</v>
       </c>
       <c r="J26" s="6"/>
-      <c r="K26" s="19" t="s">
-        <v>135</v>
+      <c r="K26" s="13" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updating notes column for 3 indicators after call with CDHD
</commit_message>
<xml_diff>
--- a/documentation/NCW Epi Dashboards_indicator information.xlsx
+++ b/documentation/NCW Epi Dashboards_indicator information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amoli\OneDrive\Documents\GitHub\ncw_dashboards\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D095E53A-2AAF-4FE5-9C03-BA83432DB145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA22FB7C-749B-4908-9C75-9F10FCD023F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="152">
   <si>
     <t>Diabetes</t>
   </si>
@@ -1189,6 +1189,15 @@
   <si>
     <t>Other Dashboard Notes</t>
   </si>
+  <si>
+    <t xml:space="preserve">Access to Physicians includes doctors, with either an MD or DO degree, who have active status, and excludes doctors who are retired, working part time, temporarily not practicing, or are not active for any other reason. Any type of doctor (primary care, gynecologist, pediatricians, psychiatrists, etc.) are counted in this indicator. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 2015, the data source for this metric reports the same air quality values for Chelan and Douglas counties (potentially because they are part of the Chelan-Douglas health district).  As a result, they are fully overlapping on the dashboard. You can check or uncheck these counties on the dashboard to see them individually.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The poverty level in the US is set by the Office of Management and Budget of the White House, and depends on a family's size and composition (number of adults and children), as well as the year to account for inflation. More information on how poverty level is determined can be found here: https://www.socialexplorer.com/data/ACS2020_5yr/metadata/?ds=ACS20_5yr&amp;table=B16009 </t>
+  </si>
 </sst>
 </file>
 
@@ -1284,7 +1293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1322,18 +1331,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1557,8 +1555,8 @@
   </sheetPr>
   <dimension ref="A1:L999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I13" zoomScale="120" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1723,7 +1721,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>42</v>
       </c>
@@ -1954,7 +1952,7 @@
       <c r="H11" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="7" t="s">
         <v>54</v>
       </c>
       <c r="J11" s="6"/>
@@ -1965,139 +1963,141 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="18" customFormat="1" ht="50.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:12" ht="50.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="4">
         <v>2022</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="16" t="s">
+      <c r="H12" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J12" s="17"/>
-      <c r="K12" s="20" t="s">
+      <c r="J12" s="6"/>
+      <c r="K12" s="13" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="18" customFormat="1" ht="63.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:12" ht="63.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="4">
         <v>2022</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J13" s="17"/>
-      <c r="K13" s="20" t="s">
+      <c r="J13" s="6"/>
+      <c r="K13" s="13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="18" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:12" ht="125" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="4">
         <v>2022</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="20" t="s">
+      <c r="J14" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="K14" s="13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="18" customFormat="1" ht="50.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+    <row r="15" spans="1:12" ht="50.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="4">
         <v>2022</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="20" t="s">
+      <c r="J15" s="6"/>
+      <c r="K15" s="13" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="46" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="100.5" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
@@ -2125,7 +2125,9 @@
       <c r="I16" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="J16" s="6"/>
+      <c r="J16" s="7" t="s">
+        <v>150</v>
+      </c>
       <c r="K16" s="13" t="s">
         <v>127</v>
       </c>
@@ -2379,7 +2381,7 @@
       <c r="C24" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="16" t="s">
         <v>147</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -2435,7 +2437,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="50.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="100.5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>21</v>
       </c>
@@ -2463,7 +2465,9 @@
       <c r="I26" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="J26" s="6"/>
+      <c r="J26" s="7" t="s">
+        <v>149</v>
+      </c>
       <c r="K26" s="13" t="s">
         <v>134</v>
       </c>

</xml_diff>